<commit_message>
Changed PCB size for cotoff
</commit_message>
<xml_diff>
--- a/CoolGirl_rev6.x/board/pickplace.xlsx
+++ b/CoolGirl_rev6.x/board/pickplace.xlsx
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -585,7 +585,7 @@
         <v>17.62</v>
       </c>
       <c r="C2" s="2">
-        <v>41.274000000000001</v>
+        <v>41.988</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -602,7 +602,7 @@
         <v>13.016</v>
       </c>
       <c r="C3" s="2">
-        <v>41.274000000000001</v>
+        <v>41.988</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -619,7 +619,7 @@
         <v>24.129000000000001</v>
       </c>
       <c r="C4" s="2">
-        <v>29.277999999999999</v>
+        <v>29.992000000000001</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -636,7 +636,7 @@
         <v>24.129000000000001</v>
       </c>
       <c r="C5" s="2">
-        <v>36.759</v>
+        <v>37.473999999999997</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
@@ -653,7 +653,7 @@
         <v>40.639000000000003</v>
       </c>
       <c r="C6" s="2">
-        <v>29.297999999999998</v>
+        <v>30.013000000000002</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
@@ -670,7 +670,7 @@
         <v>40.639000000000003</v>
       </c>
       <c r="C7" s="2">
-        <v>36.829000000000001</v>
+        <v>37.542999999999999</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
@@ -687,7 +687,7 @@
         <v>73.659000000000006</v>
       </c>
       <c r="C8" s="2">
-        <v>29.300999999999998</v>
+        <v>30.015000000000001</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -704,7 +704,7 @@
         <v>73.659000000000006</v>
       </c>
       <c r="C9" s="2">
-        <v>36.793999999999997</v>
+        <v>37.508000000000003</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
@@ -721,7 +721,7 @@
         <v>90.01</v>
       </c>
       <c r="C10" s="2">
-        <v>29.276</v>
+        <v>29.99</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
@@ -738,7 +738,7 @@
         <v>90.01</v>
       </c>
       <c r="C11" s="2">
-        <v>36.829000000000001</v>
+        <v>37.542999999999999</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>6</v>
@@ -755,7 +755,7 @@
         <v>28.495999999999999</v>
       </c>
       <c r="C12" s="2">
-        <v>64.778000000000006</v>
+        <v>65.492000000000004</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
@@ -772,7 +772,7 @@
         <v>52.069000000000003</v>
       </c>
       <c r="C13" s="2">
-        <v>28.861000000000001</v>
+        <v>29.576000000000001</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>6</v>
@@ -789,7 +789,7 @@
         <v>89.691999999999993</v>
       </c>
       <c r="C14" s="2">
-        <v>25.558</v>
+        <v>26.271999999999998</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>6</v>
@@ -806,7 +806,7 @@
         <v>88.78</v>
       </c>
       <c r="C15" s="2">
-        <v>57.188000000000002</v>
+        <v>57.902999999999999</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>6</v>
@@ -823,7 +823,7 @@
         <v>77.628</v>
       </c>
       <c r="C16" s="2">
-        <v>50.322000000000003</v>
+        <v>51.036999999999999</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>6</v>
@@ -840,7 +840,7 @@
         <v>45.719000000000001</v>
       </c>
       <c r="C17" s="2">
-        <v>57.466000000000001</v>
+        <v>58.180999999999997</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>6</v>
@@ -857,7 +857,7 @@
         <v>48.1</v>
       </c>
       <c r="C18" s="2">
-        <v>60.878999999999998</v>
+        <v>61.594000000000001</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>6</v>
@@ -874,7 +874,7 @@
         <v>53.585000000000001</v>
       </c>
       <c r="C19" s="2">
-        <v>63.56</v>
+        <v>64.274000000000001</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>6</v>
@@ -891,7 +891,7 @@
         <v>47.305999999999997</v>
       </c>
       <c r="C20" s="2">
-        <v>44.448999999999998</v>
+        <v>45.162999999999997</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>6</v>
@@ -908,7 +908,7 @@
         <v>51.116</v>
       </c>
       <c r="C21" s="2">
-        <v>40.320999999999998</v>
+        <v>41.036000000000001</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>6</v>
@@ -925,7 +925,7 @@
         <v>53.576999999999998</v>
       </c>
       <c r="C22" s="2">
-        <v>38.177999999999997</v>
+        <v>38.893000000000001</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>6</v>
@@ -942,7 +942,7 @@
         <v>68.340999999999994</v>
       </c>
       <c r="C23" s="2">
-        <v>61.911000000000001</v>
+        <v>62.625999999999998</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>6</v>
@@ -959,7 +959,7 @@
         <v>70.403999999999996</v>
       </c>
       <c r="C24" s="2">
-        <v>60.244</v>
+        <v>60.959000000000003</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>6</v>
@@ -976,7 +976,7 @@
         <v>74.055999999999997</v>
       </c>
       <c r="C25" s="2">
-        <v>56.99</v>
+        <v>57.704000000000001</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>6</v>
@@ -993,7 +993,7 @@
         <v>66.123999999999995</v>
       </c>
       <c r="C26" s="2">
-        <v>37.825000000000003</v>
+        <v>38.539000000000001</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>6</v>
@@ -1010,7 +1010,7 @@
         <v>69.69</v>
       </c>
       <c r="C27" s="2">
-        <v>41.433</v>
+        <v>42.146999999999998</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>6</v>
@@ -1027,7 +1027,7 @@
         <v>73.102999999999994</v>
       </c>
       <c r="C28" s="2">
-        <v>44.686999999999998</v>
+        <v>45.401000000000003</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>6</v>
@@ -1044,7 +1044,7 @@
         <v>99.631</v>
       </c>
       <c r="C29" s="2">
-        <v>56.536999999999999</v>
+        <v>57.250999999999998</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>6</v>
@@ -1061,7 +1061,7 @@
         <v>53.18</v>
       </c>
       <c r="C30" s="2">
-        <v>26.51</v>
+        <v>27.224</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>6</v>
@@ -1078,7 +1078,7 @@
         <v>85.296000000000006</v>
       </c>
       <c r="C31" s="2">
-        <v>57.188000000000002</v>
+        <v>57.902999999999999</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>6</v>
@@ -1095,7 +1095,7 @@
         <v>87.046000000000006</v>
       </c>
       <c r="C32" s="2">
-        <v>57.188000000000002</v>
+        <v>57.902999999999999</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>6</v>
@@ -1112,7 +1112,7 @@
         <v>52.069000000000003</v>
       </c>
       <c r="C33" s="2">
-        <v>30.765999999999998</v>
+        <v>31.481000000000002</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>6</v>
@@ -1129,7 +1129,7 @@
         <v>27.545999999999999</v>
       </c>
       <c r="C34" s="2">
-        <v>25.716000000000001</v>
+        <v>26.43</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>6</v>
@@ -1146,7 +1146,7 @@
         <v>30.402999999999999</v>
       </c>
       <c r="C35" s="2">
-        <v>25.716000000000001</v>
+        <v>26.43</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>6</v>
@@ -1163,7 +1163,7 @@
         <v>33.261000000000003</v>
       </c>
       <c r="C36" s="2">
-        <v>25.716000000000001</v>
+        <v>26.43</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>6</v>
@@ -1180,7 +1180,7 @@
         <v>36.118000000000002</v>
       </c>
       <c r="C37" s="2">
-        <v>25.716000000000001</v>
+        <v>26.43</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>6</v>
@@ -1197,7 +1197,7 @@
         <v>44.765999999999998</v>
       </c>
       <c r="C38" s="2">
-        <v>25.716000000000001</v>
+        <v>26.43</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>6</v>
@@ -1214,7 +1214,7 @@
         <v>47.941000000000003</v>
       </c>
       <c r="C39" s="2">
-        <v>25.716000000000001</v>
+        <v>26.43</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>6</v>
@@ -1231,7 +1231,7 @@
         <v>76.834000000000003</v>
       </c>
       <c r="C40" s="2">
-        <v>25.716000000000001</v>
+        <v>26.43</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>6</v>
@@ -1248,7 +1248,7 @@
         <v>79.691000000000003</v>
       </c>
       <c r="C41" s="2">
-        <v>25.716000000000001</v>
+        <v>26.431000000000001</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>6</v>
@@ -1265,7 +1265,7 @@
         <v>82.549000000000007</v>
       </c>
       <c r="C42" s="2">
-        <v>25.716000000000001</v>
+        <v>26.431000000000001</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>6</v>
@@ -1282,7 +1282,7 @@
         <v>85.406000000000006</v>
       </c>
       <c r="C43" s="2">
-        <v>25.716000000000001</v>
+        <v>26.431000000000001</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>6</v>
@@ -1299,7 +1299,7 @@
         <v>94.138000000000005</v>
       </c>
       <c r="C44" s="2">
-        <v>25.716000000000001</v>
+        <v>26.431000000000001</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>6</v>
@@ -1316,7 +1316,7 @@
         <v>96.995000000000005</v>
       </c>
       <c r="C45" s="2">
-        <v>25.716000000000001</v>
+        <v>26.431000000000001</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>6</v>
@@ -1333,7 +1333,7 @@
         <v>59.054000000000002</v>
       </c>
       <c r="C46" s="2">
-        <v>25.716000000000001</v>
+        <v>26.43</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>6</v>
@@ -1350,7 +1350,7 @@
         <v>63.499000000000002</v>
       </c>
       <c r="C47" s="2">
-        <v>25.716000000000001</v>
+        <v>26.43</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>6</v>
@@ -1367,7 +1367,7 @@
         <v>60.006</v>
       </c>
       <c r="C48" s="2">
-        <v>51.353999999999999</v>
+        <v>52.069000000000003</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>6</v>
@@ -1384,7 +1384,7 @@
         <v>15.239000000000001</v>
       </c>
       <c r="C49" s="2">
-        <v>48.734999999999999</v>
+        <v>49.448999999999998</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>6</v>
@@ -1401,7 +1401,7 @@
         <v>28.097000000000001</v>
       </c>
       <c r="C50" s="2">
-        <v>51.91</v>
+        <v>52.624000000000002</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>6</v>
@@ -1418,7 +1418,7 @@
         <v>90.724000000000004</v>
       </c>
       <c r="C51" s="2">
-        <v>48.1</v>
+        <v>48.814</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>61</v>
@@ -1435,7 +1435,7 @@
         <v>91.756</v>
       </c>
       <c r="C52" s="2">
-        <v>50.005000000000003</v>
+        <v>50.719000000000001</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>6</v>
@@ -1452,7 +1452,7 @@
         <v>31.798999999999999</v>
       </c>
       <c r="C53" s="2">
-        <v>33.131999999999998</v>
+        <v>33.847000000000001</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>6</v>
@@ -1469,7 +1469,7 @@
         <v>81.12</v>
       </c>
       <c r="C54" s="2">
-        <v>33.018999999999998</v>
+        <v>33.732999999999997</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>6</v>
@@ -1486,7 +1486,7 @@
         <v>46.146999999999998</v>
       </c>
       <c r="C55" s="2">
-        <v>33.314999999999998</v>
+        <v>34.029000000000003</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>6</v>
@@ -1503,7 +1503,7 @@
         <v>95.408000000000001</v>
       </c>
       <c r="C56" s="2">
-        <v>33.177999999999997</v>
+        <v>33.892000000000003</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>6</v>

</xml_diff>